<commit_message>
Correction des problèmes noter
</commit_message>
<xml_diff>
--- a/Tableau-Audit.xlsx
+++ b/Tableau-Audit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12575" tabRatio="198"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
@@ -318,10 +318,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -377,6 +377,124 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -385,46 +503,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -436,73 +518,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -512,22 +527,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,19 +560,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -584,163 +740,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -787,30 +787,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -841,17 +817,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -866,6 +831,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -873,138 +873,138 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1013,7 +1013,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1055,12 +1054,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1455,410 +1448,410 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.1574074074074" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="28.0555555555556" style="5" customWidth="1"/>
-    <col min="2" max="3" width="28.0555555555556" style="6" customWidth="1"/>
-    <col min="4" max="4" width="30.0555555555556" style="7" customWidth="1"/>
-    <col min="5" max="5" width="28.0555555555556" style="6" customWidth="1"/>
-    <col min="6" max="6" width="28.0555555555556" style="8" customWidth="1"/>
-    <col min="7" max="7" width="28.1111111111111" style="6"/>
+    <col min="1" max="1" width="28.0555555555556" style="4" customWidth="1"/>
+    <col min="2" max="3" width="28.0555555555556" style="5" customWidth="1"/>
+    <col min="4" max="4" width="30.0555555555556" style="6" customWidth="1"/>
+    <col min="5" max="5" width="28.0555555555556" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.0555555555556" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28.1111111111111" style="5"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24.05" customHeight="1" spans="1:7">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="151.2" spans="1:7">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="75" customHeight="1" spans="1:7">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="105" spans="1:7">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="105" spans="1:7">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="45" spans="1:7">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="14"/>
+      <c r="G12" s="13"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="15" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="14"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="13"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="45" spans="1:7">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" s="4" customFormat="1" ht="60" spans="1:7">
-      <c r="A16" s="5" t="s">
+    <row r="16" s="2" customFormat="1" ht="60" spans="1:7">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F16" s="19" t="s">
+      <c r="F16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="17" s="4" customFormat="1" ht="75" spans="1:7">
-      <c r="A17" s="5" t="s">
+    <row r="17" s="2" customFormat="1" ht="75" spans="1:7">
+      <c r="A17" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="20"/>
+      <c r="F17" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="13"/>
     </row>
-    <row r="18" s="4" customFormat="1" ht="150" spans="1:7">
-      <c r="A18" s="5" t="s">
+    <row r="18" s="2" customFormat="1" ht="150" spans="1:7">
+      <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G18" s="17" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="16" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Compression des images, extension img bmp-jpg
</commit_message>
<xml_diff>
--- a/Tableau-Audit.xlsx
+++ b/Tableau-Audit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="198"/>
+    <workbookView windowWidth="28800" windowHeight="12575" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
   <si>
     <t>Catégorie</t>
   </si>
@@ -235,7 +235,7 @@
     <t>Liens obsolète</t>
   </si>
   <si>
-    <t>Certains liens de fichier ne mènent nulle part, à supprimer</t>
+    <t>Certains liens (Bootstrap, JavaScript, CSS) de fichier ne mènent nulle part et empêche la page Contact de charger correctement</t>
   </si>
   <si>
     <t>Code Page Contact</t>
@@ -244,6 +244,9 @@
     <t>Vérifier le chemin des sources...</t>
   </si>
   <si>
+    <t>MDN - Balise link</t>
+  </si>
+  <si>
     <t>meta keywords obsolète</t>
   </si>
   <si>
@@ -265,6 +268,9 @@
     <t>Remplir les balises avec du contenu pertinent</t>
   </si>
   <si>
+    <t>MDN - Balises HTML</t>
+  </si>
+  <si>
     <t>Le menu est hors chant</t>
   </si>
   <si>
@@ -292,7 +298,7 @@
     <t>Performance</t>
   </si>
   <si>
-    <t>image inutile ou lourde</t>
+    <t>image inutile ou lourde ET sans alternative textuelle</t>
   </si>
   <si>
     <t>Certaines images peuvent être supprimées (image sous forme de texte) ou peuvent être compressées pour réduire leurs tailles</t>
@@ -302,6 +308,9 @@
   </si>
   <si>
     <t xml:space="preserve">Réduire la taille des images pour optimiser les performances et ne pas oublier d'ajouter une alternative textuelle </t>
+  </si>
+  <si>
+    <t>Kinsta - Optimisation</t>
   </si>
   <si>
     <t>Formulaire</t>
@@ -318,9 +327,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="30">
@@ -377,15 +386,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,9 +407,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -412,40 +445,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -456,9 +489,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -480,9 +513,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -504,30 +536,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,187 +569,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -769,6 +778,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -780,15 +798,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -810,8 +819,10 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -828,15 +839,6 @@
       </top>
       <bottom style="double">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -858,153 +860,160 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1054,6 +1063,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="11" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1447,8 +1462,8 @@
   <sheetPr/>
   <dimension ref="A1:G18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.1574074074074" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1708,7 +1723,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" s="2" customFormat="1" ht="45" spans="1:7">
+    <row r="12" s="2" customFormat="1" ht="75" spans="1:7">
       <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
@@ -1727,27 +1742,29 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="13"/>
+      <c r="G12" s="18" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="75" spans="1:7">
       <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="15" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="75" spans="1:7">
@@ -1755,35 +1772,37 @@
         <v>39</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D14" s="12" t="s">
         <v>42</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="F14" s="14"/>
-      <c r="G14" s="13"/>
+      <c r="G14" s="19" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="45" spans="1:7">
       <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="16" t="s">
@@ -1795,60 +1814,62 @@
         <v>7</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D16" s="12" t="s">
         <v>42</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F16" s="14" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="15" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="75" spans="1:7">
       <c r="A17" s="4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="F17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="13"/>
+      <c r="G17" s="15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="150" spans="1:7">
       <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="D18" s="12" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="16" t="s">
@@ -1871,6 +1892,9 @@
     <hyperlink ref="G15" r:id="rId1" display="Openclassroom - Accessibilité"/>
     <hyperlink ref="G16" r:id="rId4" display="Checklist-seo"/>
     <hyperlink ref="G18" r:id="rId1" display="Openclassroom - Accessibilité"/>
+    <hyperlink ref="G14" r:id="rId9" display="MDN - Balises HTML"/>
+    <hyperlink ref="G17" r:id="rId10" display="Kinsta - Optimisation"/>
+    <hyperlink ref="G12" r:id="rId11" display="MDN - Balise link"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Remplacement du fichier FontAwesome par un CDN
</commit_message>
<xml_diff>
--- a/Tableau-Audit.xlsx
+++ b/Tableau-Audit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12575" tabRatio="198"/>
+    <workbookView windowWidth="22991" windowHeight="9192" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="93">
   <si>
     <t>Catégorie</t>
   </si>
@@ -321,16 +321,31 @@
   <si>
     <t>Lier les labels au chant input et faire savoir à l'utilisateur si les données ne sont pas les bonnes, pour ça il est préférable de ne pas lui indiquer seulement via une couleur par exemple pour également avec une alternative textuelle</t>
   </si>
+  <si>
+    <t>Vulnérabilité concernant la sécurité</t>
+  </si>
+  <si>
+    <t>Les versions de Bootstrap et Jquery sont très ancienne et contiennent de nombreuse vulnérabilité</t>
+  </si>
+  <si>
+    <t>Page Contact / Page Accueil</t>
+  </si>
+  <si>
+    <t>Utiliser des versions stables pour les frameworks et librairies</t>
+  </si>
+  <si>
+    <t>Vulnérabilités Web</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -402,6 +417,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
@@ -416,22 +439,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -446,14 +461,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -463,6 +471,66 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -483,60 +551,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -569,19 +584,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -593,163 +728,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -778,15 +793,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -802,6 +808,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -813,6 +828,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -842,178 +890,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1022,6 +1037,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1069,6 +1085,9 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1460,420 +1479,441 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.1574074074074" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="28.0555555555556" style="4" customWidth="1"/>
-    <col min="2" max="3" width="28.0555555555556" style="5" customWidth="1"/>
-    <col min="4" max="4" width="30.0555555555556" style="6" customWidth="1"/>
-    <col min="5" max="5" width="28.0555555555556" style="5" customWidth="1"/>
-    <col min="6" max="6" width="28.0555555555556" style="7" customWidth="1"/>
-    <col min="7" max="7" width="28.1111111111111" style="5"/>
+    <col min="1" max="1" width="28.0555555555556" style="5" customWidth="1"/>
+    <col min="2" max="3" width="28.0555555555556" style="6" customWidth="1"/>
+    <col min="4" max="4" width="30.0555555555556" style="7" customWidth="1"/>
+    <col min="5" max="5" width="28.0555555555556" style="6" customWidth="1"/>
+    <col min="6" max="6" width="28.0555555555556" style="8" customWidth="1"/>
+    <col min="7" max="7" width="28.1111111111111" style="6"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24.05" customHeight="1" spans="1:7">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="11" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="151.2" spans="1:7">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="14" t="s">
+      <c r="F2" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="16" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="75" customHeight="1" spans="1:7">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="18" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="14"/>
-      <c r="G5" s="15" t="s">
+      <c r="F5" s="15"/>
+      <c r="G5" s="16" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="16" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="105" spans="1:7">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="13" t="s">
+      <c r="B10" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
+      <c r="F10" s="15"/>
+      <c r="G10" s="16" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="105" spans="1:7">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="15" t="s">
+      <c r="F11" s="15"/>
+      <c r="G11" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B12" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="19" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="15" t="s">
+      <c r="F13" s="15"/>
+      <c r="G13" s="16" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="14" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="19" t="s">
+      <c r="F14" s="15"/>
+      <c r="G14" s="20" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="45" spans="1:7">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="16" t="s">
+      <c r="F15" s="15"/>
+      <c r="G15" s="17" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="60" spans="1:7">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="13" t="s">
+      <c r="C16" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="14" t="s">
+      <c r="F16" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="16" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="14" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="16" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="150" spans="1:7">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="13" t="s">
+      <c r="C18" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="16" t="s">
+      <c r="F18" s="15"/>
+      <c r="G18" s="17" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="19" s="4" customFormat="1" ht="60" spans="1:7">
+      <c r="A19" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="F19" s="21"/>
+      <c r="G19" s="16" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1895,6 +1935,7 @@
     <hyperlink ref="G14" r:id="rId9" display="MDN - Balises HTML"/>
     <hyperlink ref="G17" r:id="rId10" display="Kinsta - Optimisation"/>
     <hyperlink ref="G12" r:id="rId11" display="MDN - Balise link"/>
+    <hyperlink ref="G19" r:id="rId12" display="Vulnérabilités Web"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Ajout screen de comparaison
</commit_message>
<xml_diff>
--- a/Tableau-Audit.xlsx
+++ b/Tableau-Audit.xlsx
@@ -322,10 +322,10 @@
     <t>Lier les labels au chant input et faire savoir à l'utilisateur si les données ne sont pas les bonnes, pour ça il est préférable de ne pas lui indiquer seulement via une couleur par exemple pour également avec une alternative textuelle</t>
   </si>
   <si>
-    <t>Vulnérabilité concernant la sécurité</t>
-  </si>
-  <si>
-    <t>Les versions de Bootstrap et Jquery sont très ancienne et contiennent de nombreuse vulnérabilité</t>
+    <t>Vulnérabilité concernant la sécurité, temps de chargement</t>
+  </si>
+  <si>
+    <t>Les versions de Bootstrap et Jquery sont très anciennes et contiennent de nombreuses vulnérabilités, et le temps de chargement pour ces fichiers est assez long</t>
   </si>
   <si>
     <t>Page Contact / Page Accueil</t>
@@ -417,6 +417,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -425,70 +510,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -505,15 +526,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -529,29 +552,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,115 +584,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -704,67 +764,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -811,6 +811,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -836,16 +845,33 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -864,171 +890,145 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="11" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1037,7 +1037,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1085,9 +1084,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1482,437 +1478,437 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.1574074074074" defaultRowHeight="15" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="28.0555555555556" style="5" customWidth="1"/>
-    <col min="2" max="3" width="28.0555555555556" style="6" customWidth="1"/>
-    <col min="4" max="4" width="30.0555555555556" style="7" customWidth="1"/>
-    <col min="5" max="5" width="28.0555555555556" style="6" customWidth="1"/>
-    <col min="6" max="6" width="28.0555555555556" style="8" customWidth="1"/>
-    <col min="7" max="7" width="28.1111111111111" style="6"/>
+    <col min="1" max="1" width="28.0555555555556" style="4" customWidth="1"/>
+    <col min="2" max="3" width="28.0555555555556" style="5" customWidth="1"/>
+    <col min="4" max="4" width="30.0555555555556" style="6" customWidth="1"/>
+    <col min="5" max="5" width="28.0555555555556" style="5" customWidth="1"/>
+    <col min="6" max="6" width="28.0555555555556" style="7" customWidth="1"/>
+    <col min="7" max="7" width="28.1111111111111" style="5"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="24.05" customHeight="1" spans="1:7">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="10" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" s="2" customFormat="1" ht="151.2" spans="1:7">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="15" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="13" t="s">
+      <c r="D3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" ht="75" customHeight="1" spans="1:7">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="D4" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="15"/>
-      <c r="G5" s="16" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="6" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="7" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="15" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="8" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="13" t="s">
+      <c r="D8" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="15" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="9" s="2" customFormat="1" ht="90" spans="1:7">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D9" s="13" t="s">
+      <c r="D9" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="15" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="10" s="2" customFormat="1" ht="105" spans="1:7">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="15"/>
-      <c r="G10" s="16" t="s">
+      <c r="F10" s="14"/>
+      <c r="G10" s="15" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="11" s="2" customFormat="1" ht="105" spans="1:7">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="D11" s="13" t="s">
+      <c r="D11" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E11" s="14" t="s">
+      <c r="E11" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="16" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="15" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="12" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="D12" s="13" t="s">
+      <c r="D12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="19" t="s">
+      <c r="G12" s="18" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="13" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="15"/>
-      <c r="G13" s="16" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="15" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="14" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E14" s="14" t="s">
+      <c r="E14" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="F14" s="15"/>
-      <c r="G14" s="20" t="s">
+      <c r="F14" s="14"/>
+      <c r="G14" s="19" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="15" s="2" customFormat="1" ht="45" spans="1:7">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="D15" s="13" t="s">
+      <c r="D15" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E15" s="14" t="s">
+      <c r="E15" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F15" s="15"/>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="16" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" s="2" customFormat="1" ht="60" spans="1:7">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="C16" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="D16" s="13" t="s">
+      <c r="D16" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="E16" s="14" t="s">
+      <c r="E16" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="16" t="s">
+      <c r="G16" s="15" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="17" s="2" customFormat="1" ht="75" spans="1:7">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="E17" s="14" t="s">
+      <c r="E17" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="16" t="s">
+      <c r="G17" s="15" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="18" s="2" customFormat="1" ht="150" spans="1:7">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="F18" s="15"/>
-      <c r="G18" s="17" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="16" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" s="4" customFormat="1" ht="60" spans="1:7">
-      <c r="A19" s="5" t="s">
+    <row r="19" s="2" customFormat="1" ht="105" spans="1:7">
+      <c r="A19" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="16" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="15" t="s">
         <v>92</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Ajout du rapport et de screen comparatif
</commit_message>
<xml_diff>
--- a/Tableau-Audit.xlsx
+++ b/Tableau-Audit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="22991" windowHeight="9192" tabRatio="198"/>
+    <workbookView windowWidth="23040" windowHeight="9335" tabRatio="198"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille1" sheetId="1" r:id="rId1"/>
@@ -187,7 +187,7 @@
     <t>Page d'accueil -                Page Contact</t>
   </si>
   <si>
-    <t>Utiliser un titre suffisamment claire pour identifier les différentes pages, dans l'idéal se titre ne doit pas dépasser les 65 caractères</t>
+    <t>Utiliser un titre suffisamment clair pour identifier les différentes pages, dans l'idéal se titre ne doit pas dépasser les 65 caractères</t>
   </si>
   <si>
     <t>Checklist SEO</t>
@@ -342,8 +342,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="176" formatCode="_-&quot;€&quot;* #,##0.00_-;\-&quot;€&quot;* #,##0.00_-;_-&quot;€&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="177" formatCode="_-* #,##0_-;\-&quot;€&quot;* #,##0_-;_-&quot;€&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
@@ -386,7 +386,7 @@
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -402,7 +402,7 @@
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -417,15 +417,73 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -439,77 +497,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -526,6 +513,28 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -534,24 +543,15 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -584,181 +584,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -793,6 +793,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -804,15 +815,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -845,7 +847,31 @@
       <right/>
       <top/>
       <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -864,167 +890,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="176" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="41" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1070,16 +1070,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="11" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="11" applyFont="1" applyAlignment="1">
@@ -1477,8 +1477,8 @@
   <sheetPr/>
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="28.1574074074074" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1600,7 +1600,7 @@
         <v>29</v>
       </c>
       <c r="F5" s="14"/>
-      <c r="G5" s="15" t="s">
+      <c r="G5" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1623,7 +1623,7 @@
       <c r="F6" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="15" t="s">
+      <c r="G6" s="18" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
       <c r="F7" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="18" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1669,7 +1669,7 @@
       <c r="F8" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G8" s="15" t="s">
+      <c r="G8" s="18" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1692,7 +1692,7 @@
       <c r="F9" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="15" t="s">
+      <c r="G9" s="18" t="s">
         <v>49</v>
       </c>
     </row>
@@ -1713,7 +1713,7 @@
         <v>52</v>
       </c>
       <c r="F10" s="14"/>
-      <c r="G10" s="15" t="s">
+      <c r="G10" s="18" t="s">
         <v>53</v>
       </c>
     </row>
@@ -1734,7 +1734,7 @@
         <v>56</v>
       </c>
       <c r="F11" s="14"/>
-      <c r="G11" s="15" t="s">
+      <c r="G11" s="18" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1757,7 +1757,7 @@
       <c r="F12" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="15" t="s">
         <v>62</v>
       </c>
     </row>
@@ -1778,7 +1778,7 @@
         <v>65</v>
       </c>
       <c r="F13" s="14"/>
-      <c r="G13" s="15" t="s">
+      <c r="G13" s="18" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1843,7 +1843,7 @@
       <c r="F16" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="18" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       <c r="F17" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="18" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1908,13 +1908,12 @@
         <v>91</v>
       </c>
       <c r="F19" s="14"/>
-      <c r="G19" s="15" t="s">
+      <c r="G19" s="18" t="s">
         <v>92</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="G2" location="Feuille1!G2" display="Expert Référencement"/>
     <hyperlink ref="G3" r:id="rId1" display="Openclassroom - Accessibilité"/>
     <hyperlink ref="G4" r:id="rId1" display="Orange Accessibilité"/>
     <hyperlink ref="G5" r:id="rId2" display="FormationVidéo - Youtube"/>
@@ -1932,6 +1931,7 @@
     <hyperlink ref="G17" r:id="rId10" display="Kinsta - Optimisation"/>
     <hyperlink ref="G12" r:id="rId11" display="MDN - Balise link"/>
     <hyperlink ref="G19" r:id="rId12" display="Vulnérabilités Web"/>
+    <hyperlink ref="G2" r:id="rId13" display="Expert Référencement"/>
   </hyperlinks>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>